<commit_message>
trying out the agent growth
</commit_message>
<xml_diff>
--- a/data/relationships/relative_preferences.xlsx
+++ b/data/relationships/relative_preferences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanda\Work\spatial_computing\data\relationships\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cobyb\Desktop\Desktop icons\Minor Spatial Computing\Github Tan\spatial_computing\data\relationships\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE0B580-9B7D-45AE-9BF9-87BAC0897E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA76D11-48A8-44A5-ADAB-A4953C4E713D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8385FF60-FA25-4234-BC55-F180054B2F53}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8385FF60-FA25-4234-BC55-F180054B2F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>sunlight_access</t>
   </si>
@@ -57,19 +57,10 @@
     <t>student_housing</t>
   </si>
   <si>
-    <t>co_cooking_A</t>
-  </si>
-  <si>
     <t>assisted_living</t>
   </si>
   <si>
-    <t>co_cooking_B</t>
-  </si>
-  <si>
     <t>starter_housing</t>
-  </si>
-  <si>
-    <t>co_cooking_C</t>
   </si>
   <si>
     <t>co_working</t>
@@ -812,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691859B3-309C-4810-BC4D-A39C70B98C25}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,10 +824,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
@@ -857,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J1" s="16"/>
     </row>
@@ -866,28 +857,28 @@
         <v>6</v>
       </c>
       <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="17">
         <v>1</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H2" s="17">
-        <v>0.9</v>
-      </c>
       <c r="I2" s="17">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="J2" s="16"/>
     </row>
@@ -896,28 +887,28 @@
         <v>7</v>
       </c>
       <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.5</v>
-      </c>
       <c r="H3" s="18">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I3" s="18">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="J3" s="16"/>
     </row>
@@ -926,25 +917,25 @@
         <v>8</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="G4" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H4" s="18">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="18">
         <v>0</v>
@@ -956,25 +947,25 @@
         <v>9</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="18">
         <v>0.7</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="18">
-        <v>0.8</v>
       </c>
       <c r="I5" s="18">
         <v>0</v>
@@ -986,28 +977,28 @@
         <v>10</v>
       </c>
       <c r="B6" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E6" s="8">
         <v>0</v>
       </c>
       <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
         <v>0.7</v>
       </c>
-      <c r="G6" s="8">
-        <v>0.8</v>
-      </c>
       <c r="H6" s="18">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="I6" s="18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="16"/>
     </row>
@@ -1016,28 +1007,28 @@
         <v>11</v>
       </c>
       <c r="B7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="8">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="E7" s="8">
         <v>0</v>
       </c>
       <c r="F7" s="8">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="G7" s="8">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H7" s="18">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="J7" s="16"/>
     </row>
@@ -1046,25 +1037,25 @@
         <v>12</v>
       </c>
       <c r="B8" s="7">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="C8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E8" s="8">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="8">
         <v>0</v>
       </c>
       <c r="H8" s="18">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I8" s="18">
         <v>0</v>
@@ -1076,19 +1067,19 @@
         <v>13</v>
       </c>
       <c r="B9" s="7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F9" s="8">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="8">
         <v>0</v>
@@ -1097,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="18">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J9" s="16"/>
     </row>
@@ -1106,19 +1097,19 @@
         <v>14</v>
       </c>
       <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
         <v>0.3</v>
       </c>
-      <c r="C10" s="8">
-        <v>0.6</v>
-      </c>
       <c r="D10" s="8">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E10" s="8">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="F10" s="8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="8">
         <v>0</v>
@@ -1136,19 +1127,19 @@
         <v>15</v>
       </c>
       <c r="B11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="E11" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="F11" s="8">
         <v>0.5</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
@@ -1166,16 +1157,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D12" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -1199,13 +1190,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="8">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="D13" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="8">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -1226,19 +1217,19 @@
         <v>18</v>
       </c>
       <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="8">
-        <v>1</v>
-      </c>
-      <c r="D14" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0.7</v>
-      </c>
       <c r="F14" s="8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G14" s="8">
         <v>0</v>
@@ -1256,25 +1247,25 @@
         <v>19</v>
       </c>
       <c r="B15" s="7">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1</v>
+      </c>
+      <c r="F15" s="8">
         <v>0.3</v>
       </c>
-      <c r="C15" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="18">
         <v>0.2</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0</v>
       </c>
       <c r="I15" s="18">
         <v>0</v>
@@ -1292,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="8">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E16" s="8">
         <v>1</v>
@@ -1316,25 +1307,25 @@
         <v>21</v>
       </c>
       <c r="B17" s="7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C17" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D17" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E17" s="8">
         <v>1</v>
       </c>
       <c r="F17" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G17" s="8">
         <v>0</v>
       </c>
       <c r="H17" s="18">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="I17" s="18">
         <v>0</v>
@@ -1346,25 +1337,25 @@
         <v>22</v>
       </c>
       <c r="B18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
       </c>
       <c r="D18" s="8">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="E18" s="8">
         <v>1</v>
       </c>
       <c r="F18" s="8">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G18" s="8">
         <v>0</v>
       </c>
       <c r="H18" s="18">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I18" s="18">
         <v>0</v>
@@ -1376,25 +1367,25 @@
         <v>23</v>
       </c>
       <c r="B19" s="7">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C19" s="8">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D19" s="8">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E19" s="8">
         <v>1</v>
       </c>
       <c r="F19" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G19" s="8">
         <v>0</v>
       </c>
       <c r="H19" s="18">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I19" s="18">
         <v>0</v>
@@ -1406,25 +1397,25 @@
         <v>24</v>
       </c>
       <c r="B20" s="7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D20" s="8">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E20" s="8">
         <v>1</v>
       </c>
       <c r="F20" s="8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="8">
         <v>0</v>
       </c>
       <c r="H20" s="18">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I20" s="18">
         <v>0</v>
@@ -1436,25 +1427,25 @@
         <v>25</v>
       </c>
       <c r="B21" s="7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D21" s="8">
         <v>0.3</v>
       </c>
       <c r="E21" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G21" s="8">
         <v>0</v>
       </c>
       <c r="H21" s="18">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="I21" s="18">
         <v>0</v>
@@ -1466,180 +1457,90 @@
         <v>26</v>
       </c>
       <c r="B22" s="7">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0</v>
+      </c>
+      <c r="C23" s="20">
+        <v>0</v>
+      </c>
+      <c r="D23" s="20">
         <v>0.4</v>
       </c>
-      <c r="D22" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="E22" s="8">
-        <v>1</v>
-      </c>
-      <c r="F22" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-      <c r="H22" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="I22" s="18">
-        <v>0</v>
-      </c>
-      <c r="J22" s="16"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="7">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
-        <v>1</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="18">
-        <v>0</v>
-      </c>
-      <c r="I23" s="18">
+      <c r="E23" s="20">
+        <v>0</v>
+      </c>
+      <c r="F23" s="20">
+        <v>0</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0</v>
+      </c>
+      <c r="H23" s="21">
+        <v>0</v>
+      </c>
+      <c r="I23" s="21">
         <v>0</v>
       </c>
       <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="C24" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="D24" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
-      <c r="H24" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="I24" s="18">
-        <v>0</v>
-      </c>
-      <c r="J24" s="16"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="7">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8">
-        <v>0</v>
-      </c>
-      <c r="D25" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="8">
-        <v>0</v>
-      </c>
-      <c r="F25" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G25" s="8">
-        <v>0</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="19">
-        <v>0</v>
-      </c>
-      <c r="C26" s="20">
-        <v>0</v>
-      </c>
-      <c r="D26" s="20">
-        <v>0.4</v>
-      </c>
-      <c r="E26" s="20">
-        <v>0</v>
-      </c>
-      <c r="F26" s="20">
-        <v>0</v>
-      </c>
-      <c r="G26" s="20">
-        <v>0</v>
-      </c>
-      <c r="H26" s="21">
-        <v>0</v>
-      </c>
-      <c r="I26" s="21">
-        <v>0</v>
-      </c>
-      <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>